<commit_message>
[CREATE TRACKER OBJECT] Created user tracker model
</commit_message>
<xml_diff>
--- a/tracker_model_example.xlsx
+++ b/tracker_model_example.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Proyectos_y_cursos\Proyectos\mancaperros_App\mancaperros_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B814DA5-51E7-4C2C-AC85-0640898661F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB1D9FF0-5079-46E2-93A9-B25F167E96F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,11 +472,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B99090A-4E31-4A46-9947-BC5E54FFC4BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,5 +783,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[FINALIZAR RUTINA] End routine button functionality added
</commit_message>
<xml_diff>
--- a/tracker_model_example.xlsx
+++ b/tracker_model_example.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Proyectos_y_cursos\Proyectos\mancaperros_App\mancaperros_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\proyectos\mancaperros_app\code\backend\mancaperros_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA7236-C573-43B5-9946-49187F6C14FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
     <t>datetime</t>
   </si>
@@ -53,9 +45,6 @@
     <t>chest</t>
   </si>
   <si>
-    <t>circuit</t>
-  </si>
-  <si>
     <t>back</t>
   </si>
   <si>
@@ -65,12 +54,6 @@
     <t>legs</t>
   </si>
   <si>
-    <t>anaerobic</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>exercise_increments</t>
   </si>
   <si>
@@ -101,25 +84,49 @@
     <t>isometric_increment</t>
   </si>
   <si>
-    <t>push_increment_units</t>
-  </si>
-  <si>
     <t>Interger</t>
   </si>
   <si>
     <t>Time (seconds)</t>
   </si>
   <si>
-    <t>Time (minutes)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Input JSON</t>
+  </si>
+  <si>
+    <t>field name</t>
+  </si>
+  <si>
+    <t>field description</t>
+  </si>
+  <si>
+    <t>exercises_summary</t>
+  </si>
+  <si>
+    <t>[exercise_plan_id]</t>
+  </si>
+  <si>
+    <t>{routine_group: chest, exercise_reps: {"push-ups": 20, "muscle-up":5}}</t>
+  </si>
+  <si>
+    <t>push_time_increment</t>
+  </si>
+  <si>
+    <t>pull_time_increment</t>
+  </si>
+  <si>
+    <t>isometric_time_increment</t>
+  </si>
+  <si>
+    <t>exercise_plan_end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +146,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,10 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,25 +500,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -504,30 +533,30 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -536,249 +565,282 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K14" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[SUMMARY BUTTON] Added front and backend development
</commit_message>
<xml_diff>
--- a/tracker_model_example.xlsx
+++ b/tracker_model_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\proyectos\mancaperros_app\code\backend\mancaperros_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA7236-C573-43B5-9946-49187F6C14FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC41E5E-9F45-4864-9CBE-C50C0C03F7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>info_type</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>exercise_plan_end</t>
+  </si>
+  <si>
+    <t>record_datetime</t>
   </si>
 </sst>
 </file>
@@ -504,12 +504,12 @@
   <dimension ref="B3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
@@ -524,323 +524,323 @@
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>